<commit_message>
mls longwave H2O. download links for all summary tables. refactor main scripts
</commit_message>
<xml_diff>
--- a/longwave/longwave_mls_H2O_total.xlsx
+++ b/longwave/longwave_mls_H2O_total.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
   <si>
     <t>pressure</t>
   </si>
@@ -31,28 +31,43 @@
     <t>cooling_rate</t>
   </si>
   <si>
+    <t>CRD</t>
+  </si>
+  <si>
+    <t>LBLRTM - CLIRAD 96</t>
+  </si>
+  <si>
+    <t>LBLRTM</t>
+  </si>
+  <si>
+    <t>RRTMG - CLIRAD</t>
+  </si>
+  <si>
+    <t>RRTMG</t>
+  </si>
+  <si>
+    <t>RRTMG - CLIRAD 96</t>
+  </si>
+  <si>
+    <t>CLIRAD</t>
+  </si>
+  <si>
+    <t>CLIRAD - CLIRAD 96</t>
+  </si>
+  <si>
+    <t>CLIRAD 96</t>
+  </si>
+  <si>
     <t>CRD - LBLRTM</t>
   </si>
   <si>
-    <t>LBLRTM - CLIRAD 96</t>
-  </si>
-  <si>
     <t>CRD - RRTMG</t>
   </si>
   <si>
-    <t>RRTMG - CLIRAD</t>
-  </si>
-  <si>
     <t>CRD - CLIRAD</t>
   </si>
   <si>
-    <t>RRTMG - CLIRAD 96</t>
-  </si>
-  <si>
     <t>CRD - CLIRAD 96</t>
-  </si>
-  <si>
-    <t>CLIRAD - CLIRAD 96</t>
   </si>
   <si>
     <t>LBLRTM - RRTMG</t>
@@ -416,7 +431,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G31"/>
+  <dimension ref="A1:G46"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -447,16 +462,16 @@
         <v>70</v>
       </c>
       <c r="C2">
-        <v>1.70000000000005e-05</v>
+        <v>0.002417</v>
       </c>
       <c r="D2">
-        <v>-0.309157020504585</v>
+        <v>-335.485371190243</v>
       </c>
       <c r="E2">
         <v>0</v>
       </c>
       <c r="F2">
-        <v>-0.309157020504585</v>
+        <v>-335.485371190243</v>
       </c>
       <c r="G2">
         <v>0</v>
@@ -468,19 +483,19 @@
         <v>30</v>
       </c>
       <c r="C3">
-        <v>0</v>
+        <v>299.8</v>
       </c>
       <c r="D3">
-        <v>-0.210490113640731</v>
+        <v>-340.015794666801</v>
       </c>
       <c r="E3">
-        <v>-0.192504242700462</v>
+        <v>30.9128228681901</v>
       </c>
       <c r="F3">
-        <v>-0.402994356339661</v>
+        <v>-309.10297179861</v>
       </c>
       <c r="G3">
-        <v>0.131545450849698</v>
+        <v>2.22966252682521</v>
       </c>
     </row>
     <row r="4" spans="1:7">
@@ -489,19 +504,19 @@
         <v>0</v>
       </c>
       <c r="C4">
-        <v>0</v>
+        <v>1013</v>
       </c>
       <c r="D4">
-        <v>-0.129530398197176</v>
+        <v>-423.662018470503</v>
       </c>
       <c r="E4">
-        <v>-0.0400936993390815</v>
+        <v>272.86192163356</v>
       </c>
       <c r="F4">
-        <v>-0.169624097536598</v>
+        <v>-150.800096836943</v>
       </c>
       <c r="G4">
-        <v>0.0446744596373336</v>
+        <v>1.81115134335482</v>
       </c>
     </row>
     <row r="5" spans="1:7">
@@ -512,16 +527,16 @@
         <v>70</v>
       </c>
       <c r="C5">
-        <v>-2.99999999999953e-06</v>
+        <v>0.0024</v>
       </c>
       <c r="D5">
-        <v>-1.27107119024316</v>
+        <v>-335.176214169739</v>
       </c>
       <c r="E5">
         <v>0</v>
       </c>
       <c r="F5">
-        <v>-1.27107119024316</v>
+        <v>-335.176214169739</v>
       </c>
       <c r="G5">
         <v>0</v>
@@ -533,19 +548,19 @@
         <v>30</v>
       </c>
       <c r="C6">
-        <v>0.100000000000023</v>
+        <v>299.8</v>
       </c>
       <c r="D6">
-        <v>-0.885694666800532</v>
+        <v>-339.80530455316</v>
       </c>
       <c r="E6">
-        <v>-0.235477131809855</v>
+        <v>31.1053271108906</v>
       </c>
       <c r="F6">
-        <v>-1.12117179861025</v>
+        <v>-308.699977442271</v>
       </c>
       <c r="G6">
-        <v>0.14878252682521</v>
+        <v>2.09811707597551</v>
       </c>
     </row>
     <row r="7" spans="1:7">
@@ -554,19 +569,19 @@
         <v>0</v>
       </c>
       <c r="C7">
-        <v>0</v>
+        <v>1013</v>
       </c>
       <c r="D7">
-        <v>-0.0639184705028697</v>
+        <v>-423.532488072306</v>
       </c>
       <c r="E7">
-        <v>-2.18337836644025</v>
+        <v>272.902015332899</v>
       </c>
       <c r="F7">
-        <v>-2.2472968369427</v>
+        <v>-150.630472739406</v>
       </c>
       <c r="G7">
-        <v>-0.0600386566451838</v>
+        <v>1.76647688371748</v>
       </c>
     </row>
     <row r="8" spans="1:7">
@@ -577,19 +592,19 @@
         <v>70</v>
       </c>
       <c r="C8">
-        <v>0</v>
+        <v>0.00242</v>
       </c>
       <c r="D8">
-        <v>-2.41075519024326</v>
+        <v>-334.2143</v>
       </c>
       <c r="E8">
-        <v>-0.00124102174077354</v>
+        <v>0</v>
       </c>
       <c r="F8">
-        <v>-2.41199621198399</v>
+        <v>-334.2143</v>
       </c>
       <c r="G8">
-        <v>-5.88597492136063</v>
+        <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:7">
@@ -598,19 +613,19 @@
         <v>30</v>
       </c>
       <c r="C9">
-        <v>0</v>
+        <v>299.7</v>
       </c>
       <c r="D9">
-        <v>-2.06415866680055</v>
+        <v>-339.1301</v>
       </c>
       <c r="E9">
-        <v>-0.353320957009856</v>
+        <v>31.1483</v>
       </c>
       <c r="F9">
-        <v>-2.41747962381032</v>
+        <v>-307.9818</v>
       </c>
       <c r="G9">
-        <v>0.0291821072852096</v>
+        <v>2.08088</v>
       </c>
     </row>
     <row r="10" spans="1:7">
@@ -619,19 +634,19 @@
         <v>0</v>
       </c>
       <c r="C10">
-        <v>0</v>
+        <v>1013</v>
       </c>
       <c r="D10">
-        <v>0.124169529497237</v>
+        <v>-423.5981</v>
       </c>
       <c r="E10">
-        <v>-2.68930736644029</v>
+        <v>275.0453</v>
       </c>
       <c r="F10">
-        <v>-2.56513783694263</v>
+        <v>-148.5528</v>
       </c>
       <c r="G10">
-        <v>-0.0875308176451837</v>
+        <v>1.87119</v>
       </c>
     </row>
     <row r="11" spans="1:7">
@@ -642,19 +657,19 @@
         <v>70</v>
       </c>
       <c r="C11">
-        <v>0</v>
+        <v>0.002417</v>
       </c>
       <c r="D11">
-        <v>0.381884809756798</v>
+        <v>-333.074616</v>
       </c>
       <c r="E11">
-        <v>-0.00314171168088</v>
+        <v>0.00124102174077354</v>
       </c>
       <c r="F11">
-        <v>0.378743098075972</v>
+        <v>-333.073374978259</v>
       </c>
       <c r="G11">
-        <v>-1.54851658</v>
+        <v>5.88597492136063</v>
       </c>
     </row>
     <row r="12" spans="1:7">
@@ -663,19 +678,19 @@
         <v>30</v>
       </c>
       <c r="C12">
-        <v>0</v>
+        <v>299.8</v>
       </c>
       <c r="D12">
-        <v>0.488917333199424</v>
+        <v>-337.951636</v>
       </c>
       <c r="E12">
-        <v>1.32774540379015</v>
+        <v>31.2661438252</v>
       </c>
       <c r="F12">
-        <v>1.81666273698966</v>
+        <v>-306.6854921748</v>
       </c>
       <c r="G12">
-        <v>0.127671852560209</v>
+        <v>2.20048041954</v>
       </c>
     </row>
     <row r="13" spans="1:7">
@@ -684,19 +699,19 @@
         <v>0</v>
       </c>
       <c r="C13">
-        <v>0</v>
+        <v>1013</v>
       </c>
       <c r="D13">
-        <v>0.124145529497184</v>
+        <v>-423.786188</v>
       </c>
       <c r="E13">
-        <v>4.65833663355971</v>
+        <v>275.551229</v>
       </c>
       <c r="F13">
-        <v>4.7824821630573</v>
+        <v>-148.234959</v>
       </c>
       <c r="G13">
-        <v>-0.0885470026451838</v>
+        <v>1.898682161</v>
       </c>
     </row>
     <row r="14" spans="1:7">
@@ -707,19 +722,19 @@
         <v>70</v>
       </c>
       <c r="C14">
-        <v>-2.00000000000001e-05</v>
+        <v>0.002417</v>
       </c>
       <c r="D14">
-        <v>-0.961914169738577</v>
+        <v>-335.867256</v>
       </c>
       <c r="E14">
-        <v>0</v>
+        <v>0.00314171168088</v>
       </c>
       <c r="F14">
-        <v>-0.961914169738577</v>
+        <v>-335.864114288319</v>
       </c>
       <c r="G14">
-        <v>0</v>
+        <v>1.54851658</v>
       </c>
     </row>
     <row r="15" spans="1:7">
@@ -728,19 +743,19 @@
         <v>30</v>
       </c>
       <c r="C15">
-        <v>0.100000000000023</v>
+        <v>299.8</v>
       </c>
       <c r="D15">
-        <v>-0.675204553159801</v>
+        <v>-340.504712</v>
       </c>
       <c r="E15">
-        <v>-0.042972889109393</v>
+        <v>29.5850774644</v>
       </c>
       <c r="F15">
-        <v>-0.718177442270587</v>
+        <v>-310.9196345356</v>
       </c>
       <c r="G15">
-        <v>0.0172370759755114</v>
+        <v>2.101990674265</v>
       </c>
     </row>
     <row r="16" spans="1:7">
@@ -749,19 +764,19 @@
         <v>0</v>
       </c>
       <c r="C16">
-        <v>0</v>
+        <v>1013</v>
       </c>
       <c r="D16">
-        <v>0.0656119276943059</v>
+        <v>-423.786164</v>
       </c>
       <c r="E16">
-        <v>-2.14328466710117</v>
+        <v>268.203585</v>
       </c>
       <c r="F16">
-        <v>-2.0776727394061</v>
+        <v>-155.582579</v>
       </c>
       <c r="G16">
-        <v>-0.104713116282517</v>
+        <v>1.899698346</v>
       </c>
     </row>
     <row r="17" spans="1:7">
@@ -772,19 +787,19 @@
         <v>70</v>
       </c>
       <c r="C17">
-        <v>-1.70000000000005e-05</v>
+        <v>1.70000000000005e-05</v>
       </c>
       <c r="D17">
-        <v>-2.10159816973868</v>
+        <v>-0.309157020504585</v>
       </c>
       <c r="E17">
-        <v>-0.00124102174077354</v>
+        <v>0</v>
       </c>
       <c r="F17">
-        <v>-2.1028391914794</v>
+        <v>-0.309157020504585</v>
       </c>
       <c r="G17">
-        <v>-5.88597492136063</v>
+        <v>0</v>
       </c>
     </row>
     <row r="18" spans="1:7">
@@ -796,16 +811,16 @@
         <v>0</v>
       </c>
       <c r="D18">
-        <v>-1.85366855315982</v>
+        <v>-0.210490113640731</v>
       </c>
       <c r="E18">
-        <v>-0.160816714309394</v>
+        <v>-0.192504242700462</v>
       </c>
       <c r="F18">
-        <v>-2.01448526747066</v>
+        <v>-0.402994356339661</v>
       </c>
       <c r="G18">
-        <v>-0.102363343564489</v>
+        <v>0.131545450849698</v>
       </c>
     </row>
     <row r="19" spans="1:7">
@@ -817,39 +832,39 @@
         <v>0</v>
       </c>
       <c r="D19">
-        <v>0.253699927694413</v>
+        <v>-0.129530398197176</v>
       </c>
       <c r="E19">
-        <v>-2.64921366710121</v>
+        <v>-0.0400936993390815</v>
       </c>
       <c r="F19">
-        <v>-2.39551373940603</v>
+        <v>-0.169624097536598</v>
       </c>
       <c r="G19">
-        <v>-0.132205277282517</v>
+        <v>0.0446744596373336</v>
       </c>
     </row>
     <row r="20" spans="1:7">
       <c r="A20" s="1" t="s">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="B20" s="1">
         <v>70</v>
       </c>
       <c r="C20">
-        <v>-1.70000000000005e-05</v>
+        <v>-2.99999999999953e-06</v>
       </c>
       <c r="D20">
-        <v>0.691041830261383</v>
+        <v>-1.27107119024316</v>
       </c>
       <c r="E20">
-        <v>-0.00314171168088</v>
+        <v>0</v>
       </c>
       <c r="F20">
-        <v>0.687900118580558</v>
+        <v>-1.27107119024316</v>
       </c>
       <c r="G20">
-        <v>-1.54851658</v>
+        <v>0</v>
       </c>
     </row>
     <row r="21" spans="1:7">
@@ -858,19 +873,19 @@
         <v>30</v>
       </c>
       <c r="C21">
-        <v>0</v>
+        <v>0.100000000000023</v>
       </c>
       <c r="D21">
-        <v>0.699407446840155</v>
+        <v>-0.885694666800532</v>
       </c>
       <c r="E21">
-        <v>1.52024964649061</v>
+        <v>-0.235477131809855</v>
       </c>
       <c r="F21">
-        <v>2.21965709332932</v>
+        <v>-1.12117179861025</v>
       </c>
       <c r="G21">
-        <v>-0.00387359828948908</v>
+        <v>0.14878252682521</v>
       </c>
     </row>
     <row r="22" spans="1:7">
@@ -882,36 +897,36 @@
         <v>0</v>
       </c>
       <c r="D22">
-        <v>0.25367592769436</v>
+        <v>-0.0639184705028697</v>
       </c>
       <c r="E22">
-        <v>4.69843033289879</v>
+        <v>-2.18337836644025</v>
       </c>
       <c r="F22">
-        <v>4.95210626059389</v>
+        <v>-2.2472968369427</v>
       </c>
       <c r="G22">
-        <v>-0.133221462282517</v>
+        <v>-0.0600386566451838</v>
       </c>
     </row>
     <row r="23" spans="1:7">
       <c r="A23" s="1" t="s">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="B23" s="1">
         <v>70</v>
       </c>
       <c r="C23">
-        <v>2.99999999999953e-06</v>
+        <v>0</v>
       </c>
       <c r="D23">
-        <v>-1.1396840000001</v>
+        <v>-2.41075519024326</v>
       </c>
       <c r="E23">
         <v>-0.00124102174077354</v>
       </c>
       <c r="F23">
-        <v>-1.14092502174083</v>
+        <v>-2.41199621198399</v>
       </c>
       <c r="G23">
         <v>-5.88597492136063</v>
@@ -923,19 +938,19 @@
         <v>30</v>
       </c>
       <c r="C24">
-        <v>-0.100000000000023</v>
+        <v>0</v>
       </c>
       <c r="D24">
-        <v>-1.17846400000002</v>
+        <v>-2.06415866680055</v>
       </c>
       <c r="E24">
-        <v>-0.117843825200001</v>
+        <v>-0.353320957009856</v>
       </c>
       <c r="F24">
-        <v>-1.29630782520007</v>
+        <v>-2.41747962381032</v>
       </c>
       <c r="G24">
-        <v>-0.11960041954</v>
+        <v>0.0291821072852096</v>
       </c>
     </row>
     <row r="25" spans="1:7">
@@ -947,36 +962,36 @@
         <v>0</v>
       </c>
       <c r="D25">
-        <v>0.188088000000107</v>
+        <v>0.124169529497237</v>
       </c>
       <c r="E25">
-        <v>-0.505929000000037</v>
+        <v>-2.68930736644029</v>
       </c>
       <c r="F25">
-        <v>-0.31784099999993</v>
+        <v>-2.56513783694263</v>
       </c>
       <c r="G25">
-        <v>-0.0274921609999998</v>
+        <v>-0.0875308176451837</v>
       </c>
     </row>
     <row r="26" spans="1:7">
       <c r="A26" s="1" t="s">
-        <v>10</v>
+        <v>17</v>
       </c>
       <c r="B26" s="1">
         <v>70</v>
       </c>
       <c r="C26">
-        <v>2.99999999999953e-06</v>
+        <v>0</v>
       </c>
       <c r="D26">
-        <v>1.65295599999996</v>
+        <v>0.381884809756798</v>
       </c>
       <c r="E26">
         <v>-0.00314171168088</v>
       </c>
       <c r="F26">
-        <v>1.64981428831913</v>
+        <v>0.378743098075972</v>
       </c>
       <c r="G26">
         <v>-1.54851658</v>
@@ -988,19 +1003,19 @@
         <v>30</v>
       </c>
       <c r="C27">
-        <v>-0.100000000000023</v>
+        <v>0</v>
       </c>
       <c r="D27">
-        <v>1.37461199999996</v>
+        <v>0.488917333199424</v>
       </c>
       <c r="E27">
-        <v>1.5632225356</v>
+        <v>1.32774540379015</v>
       </c>
       <c r="F27">
-        <v>2.9378345355999</v>
+        <v>1.81666273698966</v>
       </c>
       <c r="G27">
-        <v>-0.0211106742650005</v>
+        <v>0.127671852560209</v>
       </c>
     </row>
     <row r="28" spans="1:7">
@@ -1012,39 +1027,39 @@
         <v>0</v>
       </c>
       <c r="D28">
-        <v>0.188064000000054</v>
+        <v>0.124145529497184</v>
       </c>
       <c r="E28">
-        <v>6.84171499999997</v>
+        <v>4.65833663355971</v>
       </c>
       <c r="F28">
-        <v>7.02977899999999</v>
+        <v>4.7824821630573</v>
       </c>
       <c r="G28">
-        <v>-0.028508346</v>
+        <v>-0.0885470026451838</v>
       </c>
     </row>
     <row r="29" spans="1:7">
       <c r="A29" s="1" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="B29" s="1">
         <v>70</v>
       </c>
       <c r="C29">
-        <v>0</v>
+        <v>-2.00000000000001e-05</v>
       </c>
       <c r="D29">
-        <v>2.79264000000006</v>
+        <v>-0.961914169738577</v>
       </c>
       <c r="E29">
-        <v>-0.00190068994010646</v>
+        <v>0</v>
       </c>
       <c r="F29">
-        <v>2.79073931005996</v>
+        <v>-0.961914169738577</v>
       </c>
       <c r="G29">
-        <v>4.33745834136063</v>
+        <v>0</v>
       </c>
     </row>
     <row r="30" spans="1:7">
@@ -1053,19 +1068,19 @@
         <v>30</v>
       </c>
       <c r="C30">
-        <v>0</v>
+        <v>0.100000000000023</v>
       </c>
       <c r="D30">
-        <v>2.55307599999998</v>
+        <v>-0.675204553159801</v>
       </c>
       <c r="E30">
-        <v>1.6810663608</v>
+        <v>-0.042972889109393</v>
       </c>
       <c r="F30">
-        <v>4.23414236079998</v>
+        <v>-0.718177442270587</v>
       </c>
       <c r="G30">
-        <v>0.0984897452749998</v>
+        <v>0.0172370759755114</v>
       </c>
     </row>
     <row r="31" spans="1:7">
@@ -1077,30 +1092,360 @@
         <v>0</v>
       </c>
       <c r="D31">
+        <v>0.0656119276943059</v>
+      </c>
+      <c r="E31">
+        <v>-2.14328466710117</v>
+      </c>
+      <c r="F31">
+        <v>-2.0776727394061</v>
+      </c>
+      <c r="G31">
+        <v>-0.104713116282517</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7">
+      <c r="A32" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B32" s="1">
+        <v>70</v>
+      </c>
+      <c r="C32">
+        <v>-1.70000000000005e-05</v>
+      </c>
+      <c r="D32">
+        <v>-2.10159816973868</v>
+      </c>
+      <c r="E32">
+        <v>-0.00124102174077354</v>
+      </c>
+      <c r="F32">
+        <v>-2.1028391914794</v>
+      </c>
+      <c r="G32">
+        <v>-5.88597492136063</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7">
+      <c r="A33" s="1"/>
+      <c r="B33" s="1">
+        <v>30</v>
+      </c>
+      <c r="C33">
+        <v>0</v>
+      </c>
+      <c r="D33">
+        <v>-1.85366855315982</v>
+      </c>
+      <c r="E33">
+        <v>-0.160816714309394</v>
+      </c>
+      <c r="F33">
+        <v>-2.01448526747066</v>
+      </c>
+      <c r="G33">
+        <v>-0.102363343564489</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7">
+      <c r="A34" s="1"/>
+      <c r="B34" s="1">
+        <v>0</v>
+      </c>
+      <c r="C34">
+        <v>0</v>
+      </c>
+      <c r="D34">
+        <v>0.253699927694413</v>
+      </c>
+      <c r="E34">
+        <v>-2.64921366710121</v>
+      </c>
+      <c r="F34">
+        <v>-2.39551373940603</v>
+      </c>
+      <c r="G34">
+        <v>-0.132205277282517</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7">
+      <c r="A35" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B35" s="1">
+        <v>70</v>
+      </c>
+      <c r="C35">
+        <v>-1.70000000000005e-05</v>
+      </c>
+      <c r="D35">
+        <v>0.691041830261383</v>
+      </c>
+      <c r="E35">
+        <v>-0.00314171168088</v>
+      </c>
+      <c r="F35">
+        <v>0.687900118580558</v>
+      </c>
+      <c r="G35">
+        <v>-1.54851658</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7">
+      <c r="A36" s="1"/>
+      <c r="B36" s="1">
+        <v>30</v>
+      </c>
+      <c r="C36">
+        <v>0</v>
+      </c>
+      <c r="D36">
+        <v>0.699407446840155</v>
+      </c>
+      <c r="E36">
+        <v>1.52024964649061</v>
+      </c>
+      <c r="F36">
+        <v>2.21965709332932</v>
+      </c>
+      <c r="G36">
+        <v>-0.00387359828948908</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7">
+      <c r="A37" s="1"/>
+      <c r="B37" s="1">
+        <v>0</v>
+      </c>
+      <c r="C37">
+        <v>0</v>
+      </c>
+      <c r="D37">
+        <v>0.25367592769436</v>
+      </c>
+      <c r="E37">
+        <v>4.69843033289879</v>
+      </c>
+      <c r="F37">
+        <v>4.95210626059389</v>
+      </c>
+      <c r="G37">
+        <v>-0.133221462282517</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7">
+      <c r="A38" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B38" s="1">
+        <v>70</v>
+      </c>
+      <c r="C38">
+        <v>2.99999999999953e-06</v>
+      </c>
+      <c r="D38">
+        <v>-1.1396840000001</v>
+      </c>
+      <c r="E38">
+        <v>-0.00124102174077354</v>
+      </c>
+      <c r="F38">
+        <v>-1.14092502174083</v>
+      </c>
+      <c r="G38">
+        <v>-5.88597492136063</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7">
+      <c r="A39" s="1"/>
+      <c r="B39" s="1">
+        <v>30</v>
+      </c>
+      <c r="C39">
+        <v>-0.100000000000023</v>
+      </c>
+      <c r="D39">
+        <v>-1.17846400000002</v>
+      </c>
+      <c r="E39">
+        <v>-0.117843825200001</v>
+      </c>
+      <c r="F39">
+        <v>-1.29630782520007</v>
+      </c>
+      <c r="G39">
+        <v>-0.11960041954</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7">
+      <c r="A40" s="1"/>
+      <c r="B40" s="1">
+        <v>0</v>
+      </c>
+      <c r="C40">
+        <v>0</v>
+      </c>
+      <c r="D40">
+        <v>0.188088000000107</v>
+      </c>
+      <c r="E40">
+        <v>-0.505929000000037</v>
+      </c>
+      <c r="F40">
+        <v>-0.31784099999993</v>
+      </c>
+      <c r="G40">
+        <v>-0.0274921609999998</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7">
+      <c r="A41" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B41" s="1">
+        <v>70</v>
+      </c>
+      <c r="C41">
+        <v>2.99999999999953e-06</v>
+      </c>
+      <c r="D41">
+        <v>1.65295599999996</v>
+      </c>
+      <c r="E41">
+        <v>-0.00314171168088</v>
+      </c>
+      <c r="F41">
+        <v>1.64981428831913</v>
+      </c>
+      <c r="G41">
+        <v>-1.54851658</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7">
+      <c r="A42" s="1"/>
+      <c r="B42" s="1">
+        <v>30</v>
+      </c>
+      <c r="C42">
+        <v>-0.100000000000023</v>
+      </c>
+      <c r="D42">
+        <v>1.37461199999996</v>
+      </c>
+      <c r="E42">
+        <v>1.5632225356</v>
+      </c>
+      <c r="F42">
+        <v>2.9378345355999</v>
+      </c>
+      <c r="G42">
+        <v>-0.0211106742650005</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7">
+      <c r="A43" s="1"/>
+      <c r="B43" s="1">
+        <v>0</v>
+      </c>
+      <c r="C43">
+        <v>0</v>
+      </c>
+      <c r="D43">
+        <v>0.188064000000054</v>
+      </c>
+      <c r="E43">
+        <v>6.84171499999997</v>
+      </c>
+      <c r="F43">
+        <v>7.02977899999999</v>
+      </c>
+      <c r="G43">
+        <v>-0.028508346</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7">
+      <c r="A44" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B44" s="1">
+        <v>70</v>
+      </c>
+      <c r="C44">
+        <v>0</v>
+      </c>
+      <c r="D44">
+        <v>2.79264000000006</v>
+      </c>
+      <c r="E44">
+        <v>-0.00190068994010646</v>
+      </c>
+      <c r="F44">
+        <v>2.79073931005996</v>
+      </c>
+      <c r="G44">
+        <v>4.33745834136063</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7">
+      <c r="A45" s="1"/>
+      <c r="B45" s="1">
+        <v>30</v>
+      </c>
+      <c r="C45">
+        <v>0</v>
+      </c>
+      <c r="D45">
+        <v>2.55307599999998</v>
+      </c>
+      <c r="E45">
+        <v>1.6810663608</v>
+      </c>
+      <c r="F45">
+        <v>4.23414236079998</v>
+      </c>
+      <c r="G45">
+        <v>0.0984897452749998</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7">
+      <c r="A46" s="1"/>
+      <c r="B46" s="1">
+        <v>0</v>
+      </c>
+      <c r="C46">
+        <v>0</v>
+      </c>
+      <c r="D46">
         <v>-2.40000000530927e-05</v>
       </c>
-      <c r="E31">
+      <c r="E46">
         <v>7.347644</v>
       </c>
-      <c r="F31">
+      <c r="F46">
         <v>7.34761999999992</v>
       </c>
-      <c r="G31">
+      <c r="G46">
         <v>-0.00101618500000011</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="10">
+  <mergeCells count="15">
     <mergeCell ref="A2:A4"/>
-    <mergeCell ref="A20:A22"/>
+    <mergeCell ref="A35:A37"/>
     <mergeCell ref="A5:A7"/>
-    <mergeCell ref="A23:A25"/>
+    <mergeCell ref="A38:A40"/>
     <mergeCell ref="A8:A10"/>
-    <mergeCell ref="A26:A28"/>
+    <mergeCell ref="A41:A43"/>
     <mergeCell ref="A11:A13"/>
-    <mergeCell ref="A29:A31"/>
+    <mergeCell ref="A44:A46"/>
     <mergeCell ref="A14:A16"/>
     <mergeCell ref="A17:A19"/>
+    <mergeCell ref="A20:A22"/>
+    <mergeCell ref="A23:A25"/>
+    <mergeCell ref="A26:A28"/>
+    <mergeCell ref="A29:A31"/>
+    <mergeCell ref="A32:A34"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>